<commit_message>
downloaded a lot more files
</commit_message>
<xml_diff>
--- a/parts list.xlsx
+++ b/parts list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naich\Desktop\2PPoggers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9986CE20-2B82-43D6-883E-85FBC8F84A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76D092F-C649-4A58-82C3-C48BEE72A887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="30940" windowHeight="18700" xr2:uid="{EC5D611D-8712-45C9-A383-EF55E57F7C25}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{EC5D611D-8712-45C9-A383-EF55E57F7C25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
   <si>
     <t>Part Number</t>
   </si>
@@ -224,6 +224,42 @@
   </si>
   <si>
     <t>Cerna Microscope Body 500mm Rail</t>
+  </si>
+  <si>
+    <t>KM200V</t>
+  </si>
+  <si>
+    <t>halfplate</t>
+  </si>
+  <si>
+    <t>halfplate stand</t>
+  </si>
+  <si>
+    <t>PBS10780</t>
+  </si>
+  <si>
+    <t>beam splitter</t>
+  </si>
+  <si>
+    <t>apperature stop (absorb light)</t>
+  </si>
+  <si>
+    <t>black pannel'</t>
+  </si>
+  <si>
+    <t>half-plate --&gt; beam splitter --&gt; Apperature stop --&gt; Galvo --&gt; scanning lens (SL50) --&gt; tube lens (TTL200) --&gt; x50 NIR objective</t>
+  </si>
+  <si>
+    <t>NIR objective 50x</t>
+  </si>
+  <si>
+    <t>good luck have fun</t>
+  </si>
+  <si>
+    <t>dichroic mirror - 45deg slant</t>
+  </si>
+  <si>
+    <t>EO-PC-850</t>
   </si>
 </sst>
 </file>
@@ -447,7 +483,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -465,6 +501,16 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -797,22 +843,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C18B46-1EDA-4A1C-8180-DDFB14903E5D}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:AO41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" style="3" customWidth="1"/>
     <col min="2" max="2" width="60" style="5" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="19.54296875" style="5" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="2"/>
+    <col min="3" max="3" width="13.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" style="5" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -826,15 +872,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.4">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:4" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="22"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="28"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -844,15 +890,15 @@
       <c r="C3" s="8"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="19"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="25"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -860,7 +906,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
@@ -870,15 +916,15 @@
       <c r="C6" s="11"/>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="17" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="25"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -887,7 +933,7 @@
       </c>
       <c r="C8" s="16"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -895,7 +941,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -904,7 +950,7 @@
       </c>
       <c r="C10" s="16"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -912,7 +958,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -920,7 +966,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -929,15 +975,15 @@
       </c>
       <c r="C13" s="16"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="17" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="19"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="25"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>25</v>
       </c>
@@ -945,7 +991,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
@@ -953,15 +999,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="17" t="s">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A17" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="19"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="25"/>
+    </row>
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>31</v>
       </c>
@@ -969,8 +1015,11 @@
         <v>34</v>
       </c>
       <c r="C18" s="16"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D18" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>32</v>
       </c>
@@ -979,7 +1028,7 @@
       </c>
       <c r="C19" s="16"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>33</v>
       </c>
@@ -988,15 +1037,15 @@
       </c>
       <c r="C20" s="16"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="17" t="s">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A21" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="19"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="25"/>
+    </row>
+    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>38</v>
       </c>
@@ -1004,7 +1053,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>39</v>
       </c>
@@ -1012,15 +1061,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="17" t="s">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A24" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="19"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="25"/>
+    </row>
+    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>41</v>
       </c>
@@ -1029,7 +1078,7 @@
       </c>
       <c r="C25" s="16"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>42</v>
       </c>
@@ -1037,7 +1086,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>43</v>
       </c>
@@ -1045,23 +1094,69 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="17" t="s">
+      <c r="E28" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="22"/>
+      <c r="O28" s="22"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="22"/>
+      <c r="R28" s="22"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="22"/>
+      <c r="U28" s="22"/>
+      <c r="V28" s="22"/>
+      <c r="W28" s="22"/>
+      <c r="X28" s="22"/>
+      <c r="Y28" s="22"/>
+      <c r="Z28" s="22"/>
+      <c r="AA28" s="22"/>
+      <c r="AB28" s="22"/>
+      <c r="AC28" s="22"/>
+      <c r="AD28" s="22"/>
+      <c r="AE28" s="22"/>
+      <c r="AF28" s="22"/>
+      <c r="AG28" s="22"/>
+      <c r="AH28" s="22"/>
+      <c r="AI28" s="22"/>
+      <c r="AJ28" s="22"/>
+      <c r="AK28" s="22"/>
+      <c r="AL28" s="22"/>
+      <c r="AM28" s="22"/>
+      <c r="AN28" s="22"/>
+      <c r="AO28" s="22"/>
+    </row>
+    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A29" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="19"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+    </row>
+    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>51</v>
       </c>
@@ -1069,8 +1164,15 @@
         <v>57</v>
       </c>
       <c r="C30" s="16"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E30" s="19"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+    </row>
+    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>52</v>
       </c>
@@ -1078,8 +1180,15 @@
         <v>58</v>
       </c>
       <c r="C31" s="16"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E31" s="19"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+    </row>
+    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>53</v>
       </c>
@@ -1087,8 +1196,15 @@
         <v>59</v>
       </c>
       <c r="C32" s="16"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E32" s="19"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>54</v>
       </c>
@@ -1096,8 +1212,15 @@
         <v>60</v>
       </c>
       <c r="C33" s="16"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E33" s="19"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>55</v>
       </c>
@@ -1105,8 +1228,15 @@
         <v>61</v>
       </c>
       <c r="C34" s="16"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="E34" s="19"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="20"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>56</v>
       </c>
@@ -1114,9 +1244,58 @@
         <v>62</v>
       </c>
       <c r="C35" s="16"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" s="17"/>
+      <c r="D40" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>71</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="E28:AO28"/>
     <mergeCell ref="A24:D24"/>
     <mergeCell ref="A29:D29"/>
     <mergeCell ref="A2:D2"/>

</xml_diff>